<commit_message>
Ostatnia przed urlopem wersja, wprowadzono przeniesienie ustawień kanału enkodera z pętli GUI do pętli akwizycji
</commit_message>
<xml_diff>
--- a/Dokumantacja/KonfigZakresow.xlsx
+++ b/Dokumantacja/KonfigZakresow.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="53">
   <si>
     <t>Zakres zadany</t>
   </si>
@@ -170,6 +170,12 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>mnożnik</t>
+  </si>
+  <si>
+    <t>mnożlik - wartość wklejona</t>
   </si>
 </sst>
 </file>
@@ -1613,10 +1619,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:K20"/>
+  <dimension ref="B4:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1625,7 +1631,7 @@
     <col min="7" max="7" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:11" ht="43.5" customHeight="1">
+    <row r="4" spans="2:13" ht="43.5" customHeight="1">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
@@ -1652,8 +1658,14 @@
       <c r="K4" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="5" spans="2:11">
+      <c r="L4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13">
       <c r="D5">
         <v>1000</v>
       </c>
@@ -1677,8 +1689,15 @@
         <f>D5*H5/I5</f>
         <v>1.8647255217914906</v>
       </c>
-    </row>
-    <row r="6" spans="2:11">
+      <c r="L5">
+        <f>I5/H5</f>
+        <v>536.27195440499668</v>
+      </c>
+      <c r="M5">
+        <v>536.27195440499702</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13">
       <c r="D6">
         <v>300</v>
       </c>
@@ -1699,14 +1718,21 @@
         <v>767.42340000000002</v>
       </c>
       <c r="J6">
-        <f>D6*H6/I6</f>
+        <f t="shared" ref="J5:J12" si="1">D6*H6/I6</f>
         <v>1.8976344740074382</v>
       </c>
       <c r="K6">
         <v>1.55</v>
       </c>
-    </row>
-    <row r="7" spans="2:11">
+      <c r="L6">
+        <f t="shared" ref="L6:L12" si="2">I6/H6</f>
+        <v>158.09156300078055</v>
+      </c>
+      <c r="M6">
+        <v>158.09156300078101</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4">
@@ -1730,14 +1756,21 @@
         <v>85.287910000000011</v>
       </c>
       <c r="J7">
-        <f>D7*H7/I7</f>
+        <f t="shared" si="1"/>
         <v>1.6778861153943152</v>
       </c>
       <c r="K7">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="8" spans="2:11">
+      <c r="L7">
+        <f t="shared" si="2"/>
+        <v>59.598800587547196</v>
+      </c>
+      <c r="M7">
+        <v>59.598800587547196</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13">
       <c r="D8">
         <v>30</v>
       </c>
@@ -1759,14 +1792,21 @@
         <v>77.642340000000004</v>
       </c>
       <c r="J8">
-        <f>D8*H8/I8</f>
+        <f t="shared" si="1"/>
         <v>1.8756378285353066</v>
       </c>
       <c r="K8">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="9" spans="2:11">
+      <c r="L8">
+        <f t="shared" si="2"/>
+        <v>15.994559047375965</v>
+      </c>
+      <c r="M8">
+        <v>15.994559047376001</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4">
@@ -1789,14 +1829,21 @@
         <v>7.6455700000000002</v>
       </c>
       <c r="J9">
-        <f>D9*H9/I9</f>
+        <f t="shared" si="1"/>
         <v>1.8717165626630845</v>
       </c>
       <c r="K9">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="10" spans="2:11" ht="15">
+      <c r="L9">
+        <f t="shared" si="2"/>
+        <v>5.3426892722325263</v>
+      </c>
+      <c r="M9">
+        <v>5.3426892722325263</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" ht="15">
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10">
@@ -1819,14 +1866,21 @@
         <v>7.6455700000000002</v>
       </c>
       <c r="J10">
-        <f>D10*H10/I10</f>
+        <f t="shared" si="1"/>
         <v>1.9047488938038628</v>
       </c>
       <c r="K10">
         <v>1.45</v>
       </c>
-    </row>
-    <row r="11" spans="2:11">
+      <c r="L10">
+        <f t="shared" si="2"/>
+        <v>1.5750107585094197</v>
+      </c>
+      <c r="M10">
+        <v>1.57501075850942</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4">
@@ -1849,14 +1903,21 @@
         <v>7.6455700000000002</v>
       </c>
       <c r="J11">
-        <f>D11*H11/I11</f>
+        <f t="shared" si="1"/>
         <v>1.6399378986785811</v>
       </c>
       <c r="K11">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="12" spans="2:11">
+      <c r="L11">
+        <f t="shared" si="2"/>
+        <v>0.60977918786179264</v>
+      </c>
+      <c r="M11">
+        <v>0.60977918786179264</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13">
       <c r="D12">
         <v>0.3</v>
       </c>
@@ -1878,14 +1939,21 @@
         <v>1</v>
       </c>
       <c r="J12">
-        <f>D12*H12/I12</f>
+        <f t="shared" si="1"/>
         <v>4.1907882000000001</v>
       </c>
       <c r="K12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="2:11">
+      <c r="L12">
+        <f t="shared" si="2"/>
+        <v>7.1585579056464843E-2</v>
+      </c>
+      <c r="M12">
+        <v>7.1585579056464801E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13">
       <c r="B13" s="4">
         <v>0</v>
       </c>
@@ -1900,7 +1968,7 @@
         <v>7.0710678118654752E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:11">
+    <row r="14" spans="2:13">
       <c r="B14">
         <v>1</v>
       </c>
@@ -1908,7 +1976,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="2:11">
+    <row r="15" spans="2:13">
       <c r="B15">
         <v>2</v>
       </c>
@@ -1919,7 +1987,7 @@
         <v>77.642340000000004</v>
       </c>
     </row>
-    <row r="16" spans="2:11">
+    <row r="16" spans="2:13">
       <c r="B16">
         <v>3</v>
       </c>

</xml_diff>